<commit_message>
modify the feature of  配送质量是否完好
</commit_message>
<xml_diff>
--- a/user_data_for_haier.xlsx
+++ b/user_data_for_haier.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -275,6 +275,7 @@
         <sz val="11"/>
         <color indexed="9"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>回购该品牌</t>
@@ -285,6 +286,7 @@
         <sz val="11"/>
         <color indexed="9"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>同品类</t>
@@ -294,6 +296,7 @@
         <sz val="11"/>
         <color indexed="9"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>产品意愿</t>
@@ -305,6 +308,7 @@
         <sz val="11"/>
         <color indexed="9"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>回购</t>
@@ -315,6 +319,7 @@
         <sz val="11"/>
         <color indexed="9"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>同品牌</t>
@@ -324,6 +329,7 @@
         <sz val="11"/>
         <color indexed="9"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>产品意愿</t>
@@ -695,18 +701,21 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="18"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -714,11 +723,13 @@
       <sz val="11"/>
       <color indexed="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -1783,10 +1794,10 @@
   <dimension ref="A1:FX212"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="111" zoomScaleNormal="111" zoomScalePageLayoutView="111" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B92" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="J26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N61" sqref="N61"/>
+      <selection pane="bottomRight" activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14" zeroHeight="1" x14ac:dyDescent="0.15"/>
@@ -9315,7 +9326,7 @@
         <v>1</v>
       </c>
       <c r="N36" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O36" s="22">
         <v>1</v>
@@ -13419,7 +13430,7 @@
         <v>0</v>
       </c>
       <c r="N55" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O55" s="26">
         <v>0</v>

</xml_diff>